<commit_message>
probably the end of this project
</commit_message>
<xml_diff>
--- a/variant_validation_pool.xlsx
+++ b/variant_validation_pool.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keith_tetrad/kw_dms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AA27CA-CF07-4443-A59D-B204D915E195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85A6198-E3A1-B246-A481-5526776EE47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="8600" windowWidth="25600" windowHeight="15500" xr2:uid="{E8490156-F527-8A4C-A973-00DDACFD977D}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="24860" windowHeight="15500" activeTab="3" xr2:uid="{E8490156-F527-8A4C-A973-00DDACFD977D}"/>
   </bookViews>
   <sheets>
     <sheet name="in_all_three" sheetId="1" r:id="rId1"/>
     <sheet name="in_4U8C_and_BOTH" sheetId="2" r:id="rId2"/>
     <sheet name="in_C7_and_BOTH" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="1601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="1622">
   <si>
     <t>barcode</t>
   </si>
@@ -4841,13 +4842,76 @@
   </si>
   <si>
     <t>P109D L557L</t>
+  </si>
+  <si>
+    <t>4U8C_B1T1_func_score</t>
+  </si>
+  <si>
+    <t>4U8C_B2T2_func_score</t>
+  </si>
+  <si>
+    <t>C7_B1T2_func_score</t>
+  </si>
+  <si>
+    <t>C7_B2T1_func_score</t>
+  </si>
+  <si>
+    <t>BOTH_B1T1_func_score</t>
+  </si>
+  <si>
+    <t>BOTH_B2T1_func_score</t>
+  </si>
+  <si>
+    <t>DMSO_B1T1_count</t>
+  </si>
+  <si>
+    <t>cell_line</t>
+  </si>
+  <si>
+    <t>pKW194</t>
+  </si>
+  <si>
+    <t>pKW195</t>
+  </si>
+  <si>
+    <t>pKW196</t>
+  </si>
+  <si>
+    <t>pKW197</t>
+  </si>
+  <si>
+    <t>pKW198</t>
+  </si>
+  <si>
+    <t>pKW199</t>
+  </si>
+  <si>
+    <t>pKW200</t>
+  </si>
+  <si>
+    <t>pKW201</t>
+  </si>
+  <si>
+    <t>pKW202</t>
+  </si>
+  <si>
+    <t>pKW204</t>
+  </si>
+  <si>
+    <t>pKW205</t>
+  </si>
+  <si>
+    <t>avg_func_score</t>
+  </si>
+  <si>
+    <t>DMSO_B2T1_count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4862,8 +4926,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4873,6 +4943,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4889,11 +4971,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5230,18 +5316,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9197CC4-E9C5-8D45-88B1-170C86E5ADE0}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="241" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="64" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="1"/>
-    <col min="16" max="19" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
@@ -8095,6 +8201,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8102,9 +8209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C66B9E-98CE-D944-BBE3-5F1C4B1B471C}">
   <dimension ref="A1:U235"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8633,7 +8740,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="2">
@@ -23386,6 +23493,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -23395,7 +23503,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40370,5 +40478,758 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9D8A30-4798-9045-943B-29B09EFD94D9}">
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="18.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1621</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>1601</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>1602</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>1603</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>1604</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>1605</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>1606</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E2" s="7">
+        <v>145</v>
+      </c>
+      <c r="F2" s="7">
+        <v>98</v>
+      </c>
+      <c r="G2" s="7">
+        <v>264</v>
+      </c>
+      <c r="H2" s="7">
+        <v>283</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>1</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7">
+        <v>2</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="O2" s="7">
+        <v>-7.0324170590000001</v>
+      </c>
+      <c r="P2" s="7">
+        <v>-7.9311969260000001</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>-6.5126504650000001</v>
+      </c>
+      <c r="R2" s="7">
+        <v>-7.0300291359999996</v>
+      </c>
+      <c r="S2" s="7">
+        <v>-5.4742981329999996</v>
+      </c>
+      <c r="T2" s="7">
+        <v>-8.9771624980000002</v>
+      </c>
+      <c r="U2" s="7">
+        <f>AVERAGE(O2:T2)</f>
+        <v>-7.1596257028333339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1499</v>
+      </c>
+      <c r="E3" s="6">
+        <v>102</v>
+      </c>
+      <c r="F3" s="6">
+        <v>58</v>
+      </c>
+      <c r="G3" s="6">
+        <v>76</v>
+      </c>
+      <c r="H3" s="6">
+        <v>129</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>-7.5249333109999998</v>
+      </c>
+      <c r="P3" s="6">
+        <v>-7.7977659380000004</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>-6.7559216160000002</v>
+      </c>
+      <c r="R3" s="6">
+        <v>-7.2335625300000004</v>
+      </c>
+      <c r="S3" s="6">
+        <v>-6.9668143850000002</v>
+      </c>
+      <c r="T3" s="6">
+        <v>-6.1806958920000001</v>
+      </c>
+      <c r="U3" s="6">
+        <f t="shared" ref="U3:U12" si="0">AVERAGE(O3:T3)</f>
+        <v>-7.0766156120000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="E4" s="7">
+        <v>75</v>
+      </c>
+      <c r="F4" s="7">
+        <v>254</v>
+      </c>
+      <c r="G4" s="7">
+        <v>58</v>
+      </c>
+      <c r="H4" s="7">
+        <v>147</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="O4" s="7">
+        <v>-6.0813266590000001</v>
+      </c>
+      <c r="P4" s="7">
+        <v>-7.9862110279999996</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>-7.8866253070000001</v>
+      </c>
+      <c r="R4" s="7">
+        <v>-6.843616012</v>
+      </c>
+      <c r="S4" s="7">
+        <v>-5.5232077339999996</v>
+      </c>
+      <c r="T4" s="7">
+        <v>-6.7907493739999998</v>
+      </c>
+      <c r="U4" s="7">
+        <f t="shared" si="0"/>
+        <v>-6.8519560189999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E5">
+        <v>79</v>
+      </c>
+      <c r="F5" s="4">
+        <v>136</v>
+      </c>
+      <c r="G5" s="4">
+        <v>43</v>
+      </c>
+      <c r="H5" s="4">
+        <v>52</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="4">
+        <v>-6.1562887169999998</v>
+      </c>
+      <c r="P5" s="4">
+        <v>-6.486978401</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>-7.9854034619999998</v>
+      </c>
+      <c r="R5" s="4">
+        <v>-6.4118997709999999</v>
+      </c>
+      <c r="S5" s="4">
+        <v>-6.5981697910000001</v>
+      </c>
+      <c r="T5" s="4">
+        <v>-6.3590331329999996</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.6662955458333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>179</v>
+      </c>
+      <c r="H6" s="4">
+        <v>103</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="4">
+        <v>-7.3363237459114004</v>
+      </c>
+      <c r="P6" s="4">
+        <v>-7.4730392100714802</v>
+      </c>
+      <c r="S6" s="4">
+        <v>-6.7782048204703598</v>
+      </c>
+      <c r="T6" s="4">
+        <v>-8.4003739287839192</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.4969854263092905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7">
+        <v>216</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7">
+        <v>69</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="7">
+        <v>-8.6073954708106104</v>
+      </c>
+      <c r="P7" s="7">
+        <v>-5.8950631396664397</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7">
+        <v>-7.0492765453695698</v>
+      </c>
+      <c r="T7" s="7">
+        <v>-7.0825154982056002</v>
+      </c>
+      <c r="U7" s="7">
+        <f t="shared" si="0"/>
+        <v>-7.1585626635130541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="4">
+        <v>59</v>
+      </c>
+      <c r="H8" s="4">
+        <v>284</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="4">
+        <v>-6.7351510180089802</v>
+      </c>
+      <c r="P8" s="4">
+        <v>-8.9362858023929501</v>
+      </c>
+      <c r="S8" s="4">
+        <v>-5.1770320925679396</v>
+      </c>
+      <c r="T8" s="4">
+        <v>-7.4246214750305901</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.0682725970001155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E9">
+        <v>129</v>
+      </c>
+      <c r="H9" s="4">
+        <v>55</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <v>-7.8637352240703899</v>
+      </c>
+      <c r="P9" s="4">
+        <v>-5.5678983964129296</v>
+      </c>
+      <c r="S9" s="4">
+        <v>-7.30561629862936</v>
+      </c>
+      <c r="T9" s="4">
+        <v>-6.4719271898089499</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.8022942772304074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>720</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <v>107</v>
+      </c>
+      <c r="G10" s="6">
+        <v>66</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6">
+        <v>-7.9398313269188998</v>
+      </c>
+      <c r="R10" s="6">
+        <v>-6.8521369309686104</v>
+      </c>
+      <c r="S10" s="6">
+        <v>-6.5232077337019803</v>
+      </c>
+      <c r="T10" s="6">
+        <v>-8.8869646890877902</v>
+      </c>
+      <c r="U10" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.5505351701693204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
+        <v>89</v>
+      </c>
+      <c r="G11" s="7">
+        <v>126</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7">
+        <v>-6.4450666351693204</v>
+      </c>
+      <c r="R11" s="7">
+        <v>-7.3736740515481403</v>
+      </c>
+      <c r="S11" s="7">
+        <v>-7.2716689667060201</v>
+      </c>
+      <c r="T11" s="7">
+        <v>-7.3921999973382198</v>
+      </c>
+      <c r="U11" s="7">
+        <f t="shared" si="0"/>
+        <v>-7.1206524126904256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
+        <v>107</v>
+      </c>
+      <c r="G12" s="6">
+        <v>301</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6">
+        <v>-7.0300291358904801</v>
+      </c>
+      <c r="R12" s="6">
+        <v>-6.6394076069828802</v>
+      </c>
+      <c r="S12" s="6">
+        <v>-8.5280087199658094</v>
+      </c>
+      <c r="T12" s="6">
+        <v>-5.9771624980593696</v>
+      </c>
+      <c r="U12" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.0436519902246353</v>
+      </c>
+    </row>
+    <row r="18" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>